<commit_message>
WORKING IS DATABASE POSTGRE AND BOT
</commit_message>
<xml_diff>
--- a/Market/database.xlsx
+++ b/Market/database.xlsx
@@ -1,33 +1,80 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\coding\BulkiMarket\Market\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63288FA0-B2BC-4A1F-838C-0D436C1BD8EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="1875" yWindow="2295" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="orders" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="orders" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+  <si>
+    <t>985112026</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>косяк</t>
+  </si>
+  <si>
+    <t>89008989999</t>
+  </si>
+  <si>
+    <t>игорь</t>
+  </si>
+  <si>
+    <t>Маркелоа</t>
+  </si>
+  <si>
+    <t>Test@test.ru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Булочка с ветчиной и сыром - 34009 шт. - 2380630 руб.
+2. Булочка с овсяными хлопьями - 9 шт. - 522 руб.
+3. Булочка с сыром - 45 шт. - 2430 руб.
+</t>
+  </si>
+  <si>
+    <t>2383582</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Булочка с сыром - 45 шт. - 2430 руб.
+</t>
+  </si>
+  <si>
+    <t>2430</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -45,81 +92,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -385,47 +376,88 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I6" sqref="A5:I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Косякова 74</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>79223075565</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>86423847356.00</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">1. Булочка с укропом - 90000 шт. - 3780000 руб.
-2. Булочка с овсяными хлопьями - 5432 шт. - 315056 руб.
-3. Булочка с ветчиной и сыром - 1234567890 шт. - 86419752300 руб.
-</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>86423847356</t>
-        </is>
+    <row r="1" spans="1:9" ht="180" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" ht="180" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" ht="180" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
An email distribution system has been added. The list of buyers in the database of the admin panel. A minifix is a bug fix that could cause losses. (After payment, an item of the same name was added not to the cart as a new purchase, but to an already paid item)
</commit_message>
<xml_diff>
--- a/Market/database.xlsx
+++ b/Market/database.xlsx
@@ -1,80 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\coding\BulkiMarket\Market\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63288FA0-B2BC-4A1F-838C-0D436C1BD8EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="2295" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="30675" yWindow="2295" windowWidth="21600" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="orders" sheetId="1" r:id="rId1"/>
+    <sheet name="orders" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
-  <si>
-    <t>985112026</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>косяк</t>
-  </si>
-  <si>
-    <t>89008989999</t>
-  </si>
-  <si>
-    <t>игорь</t>
-  </si>
-  <si>
-    <t>Маркелоа</t>
-  </si>
-  <si>
-    <t>Test@test.ru</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Булочка с ветчиной и сыром - 34009 шт. - 2380630 руб.
-2. Булочка с овсяными хлопьями - 9 шт. - 522 руб.
-3. Булочка с сыром - 45 шт. - 2430 руб.
-</t>
-  </si>
-  <si>
-    <t>2383582</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3. Булочка с сыром - 45 шт. - 2430 руб.
-</t>
-  </si>
-  <si>
-    <t>2430</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -89,28 +50,90 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -376,91 +399,207 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I6" sqref="A5:I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" customWidth="1"/>
+    <col width="10" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="12" bestFit="1" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H1" s="1"/>
+    <row r="1" ht="120" customHeight="1">
+      <c r="A1" t="n">
+        <v>985112026</v>
+      </c>
+      <c r="B1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>косяк</t>
+        </is>
+      </c>
+      <c r="D1" t="n">
+        <v>89008989999</v>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>игорь</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Маркелоа</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Test@test.ru</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3. Булочка с сыром - 45 шт. - 2430 руб.
+</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2430</t>
+        </is>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H2" s="1"/>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>985112026</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>косякова 88</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>89007776653</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Ян</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Вард</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>fruzzygosman123@gmail.com</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
-    <row r="3" spans="1:9" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" t="s">
-        <v>8</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>985112026</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Автомобилистов 10</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>85554447766</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Вадик</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Лысый</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>fruzzygosman123@inbox.ru</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3. Булочка с творогом и изюмом - 543 шт. - 29865 руб.
+</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>29865</t>
+        </is>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" t="s">
-        <v>10</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>985112026</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Автомобилистов 10</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>85554447766</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Вадик</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Лысый</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>fruzzygosman123@inbox.ru</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3. Булочка с творогом и изюмом - 543 шт. - 29865 руб.
+</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>29865</t>
+        </is>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>